<commit_message>
add more error analysis
</commit_message>
<xml_diff>
--- a/bidirectional/report/1-layer/analysis.xlsx
+++ b/bidirectional/report/1-layer/analysis.xlsx
@@ -105,8 +105,8 @@
           <c:yMode val="edge"/>
           <c:x val="5.6720147806238574E-2"/>
           <c:y val="4.1975314989300516E-2"/>
-          <c:w val="0.92606796150562631"/>
-          <c:h val="0.85989535917538884"/>
+          <c:w val="0.78572804232057414"/>
+          <c:h val="0.84677810507876572"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1865,15 +1865,15 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.212036582772444"/>
-          <c:y val="0.95635245579691242"/>
-          <c:w val="0.5949389512280987"/>
-          <c:h val="3.1675711004345679E-2"/>
+          <c:x val="0.86580983748314122"/>
+          <c:y val="0.25257470656525388"/>
+          <c:w val="0.12711419935941176"/>
+          <c:h val="0.17478878069135334"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2503,15 +2503,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>437030</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>168089</xdr:rowOff>
+      <xdr:colOff>1098177</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>526677</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>44824</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>168088</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2799,7 +2799,7 @@
   <dimension ref="A1:FR3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4237,6 +4237,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>